<commit_message>
Criação das APIs do novo molelo
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -356,9 +356,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -425,6 +422,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,7 +723,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -742,19 +742,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="6:12">
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="6:12">
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="6:12" ht="15" customHeight="1">
-      <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="6:12" ht="18" customHeight="1">
       <c r="H5" s="1" t="s">
@@ -762,49 +762,49 @@
       </c>
     </row>
     <row r="6" spans="6:12" ht="22.5" customHeight="1">
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="6:12" ht="27" customHeight="1">
-      <c r="H7" s="13"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="6:12">
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="6:12" ht="42" customHeight="1">
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="6:12">
-      <c r="H10" s="13"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="6:12">
       <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -812,10 +812,10 @@
       </c>
     </row>
     <row r="12" spans="6:12">
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -823,106 +823,106 @@
       <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="K13" s="12" t="s">
+      <c r="H13" s="21"/>
+      <c r="K13" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="6:12" ht="20.25" customHeight="1">
-      <c r="G14" s="25"/>
-      <c r="H14" s="23"/>
-      <c r="K14" s="13"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="22"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="6:12" ht="23.25" customHeight="1">
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="9" t="s">
+      <c r="J15" s="18"/>
+      <c r="K15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="6:12" ht="29.25" customHeight="1">
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="20" t="s">
+      <c r="K16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="45">
-      <c r="G17" s="15"/>
-      <c r="H17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="11" t="s">
+      <c r="G17" s="14"/>
+      <c r="H17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="22.5" customHeight="1">
-      <c r="E18" s="5"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="10" t="s">
+      <c r="J18" s="18"/>
+      <c r="K18" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="42" customHeight="1">
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="K19" s="12" t="s">
+      <c r="H19" s="7"/>
+      <c r="K19" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K20" s="13"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajuste para o SQLserver
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -257,13 +257,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -285,6 +278,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,62 +395,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="135"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="135"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="135"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="135"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -747,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,40 +788,40 @@
       </c>
     </row>
     <row r="6" spans="6:13" ht="22.5" customHeight="1">
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="6:13" ht="27" customHeight="1">
-      <c r="H7" s="14"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="6:13">
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="26" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="26" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="6:13" ht="42" customHeight="1">
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="6:13">
-      <c r="H10" s="14"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="6:13">
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -832,12 +833,12 @@
       <c r="I11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="6:13">
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="20" t="s">
         <v>8</v>
       </c>
       <c r="K12" s="8" t="s">
@@ -845,21 +846,21 @@
       </c>
     </row>
     <row r="13" spans="6:13" ht="24" customHeight="1">
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="K13" s="13" t="s">
+      <c r="H13" s="22"/>
+      <c r="K13" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="6:13" ht="20.25" customHeight="1">
-      <c r="G14" s="26"/>
-      <c r="H14" s="24"/>
-      <c r="K14" s="14"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="23"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="6:13" ht="23.25" customHeight="1">
       <c r="F15" s="9" t="s">
@@ -871,39 +872,39 @@
       <c r="H15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="20"/>
+      <c r="J15" s="19"/>
       <c r="K15" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="6:13" ht="29.25" customHeight="1">
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="45">
-      <c r="G17" s="16"/>
-      <c r="H17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="18"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="17"/>
       <c r="M17" s="10" t="s">
         <v>12</v>
       </c>
@@ -916,10 +917,10 @@
       <c r="H18" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="20"/>
+      <c r="J18" s="19"/>
       <c r="K18" s="9" t="s">
         <v>28</v>
       </c>
@@ -929,27 +930,27 @@
         <v>7</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="K19" s="13" t="s">
+      <c r="K19" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="26" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="14"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:13">
       <c r="K21" s="9" t="s">

</xml_diff>

<commit_message>
Tesouro direto e ajuste
</commit_message>
<xml_diff>
--- a/Modelo.xlsx
+++ b/Modelo.xlsx
@@ -752,7 +752,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -866,7 +866,7 @@
       <c r="K14" s="14"/>
     </row>
     <row r="15" spans="6:13" ht="23.25" customHeight="1">
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -924,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="J18" s="20"/>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
       <c r="K20" s="14"/>
     </row>
     <row r="21" spans="2:13">
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="12" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>